<commit_message>
added 2 missing links for the 1N5817
</commit_message>
<xml_diff>
--- a/Clock2_0-Comp_List.xlsx
+++ b/Clock2_0-Comp_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oliwi\Desktop\Project_Ontwerpen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33E586D-D2BA-4F60-A983-897D1029E00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C75219A-DBDE-44B0-816C-2559B04EA9CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -702,6 +702,42 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -720,122 +756,86 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1221,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,13 +1268,13 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="55" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="31" t="s">
@@ -1283,48 +1283,48 @@
       <c r="E3" s="22">
         <v>15.99</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="55">
         <v>1</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="56"/>
-      <c r="I3" s="53"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="61"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="28">
         <v>11.99</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="54"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="62"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="29" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="8">
         <v>12.4</v>
       </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="55"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="63"/>
       <c r="L5" s="27"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="40" t="s">
         <v>20</v>
       </c>
@@ -1343,74 +1343,74 @@
       <c r="G6" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="53"/>
+      <c r="H6" s="61"/>
       <c r="I6" s="6"/>
       <c r="L6" s="27"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="59"/>
+      <c r="B7" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="31" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="35">
         <v>0.09</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="55">
         <v>1</v>
       </c>
-      <c r="G7" s="50" t="s">
+      <c r="G7" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="54"/>
+      <c r="H7" s="62"/>
       <c r="I7" s="11"/>
       <c r="L7" s="27"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
       <c r="D8" s="31" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="36">
         <v>0.25</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="54"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="62"/>
       <c r="I8" s="11"/>
       <c r="L8" s="27"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="34" t="s">
+      <c r="A9" s="59"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="37">
         <v>0.05</v>
       </c>
-      <c r="F9" s="45"/>
+      <c r="F9" s="57"/>
       <c r="G9" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="54"/>
+      <c r="H9" s="62"/>
       <c r="I9" s="11"/>
       <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="55" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="34" t="s">
@@ -1419,58 +1419,58 @@
       <c r="E10" s="36">
         <v>0.59</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="55">
         <v>1</v>
       </c>
       <c r="G10" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="54"/>
+      <c r="H10" s="62"/>
       <c r="I10" s="11"/>
       <c r="L10" s="27"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="44"/>
+      <c r="C11" s="56"/>
       <c r="D11" s="34" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="36">
         <v>0.27</v>
       </c>
-      <c r="F11" s="44"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="54"/>
+      <c r="H11" s="62"/>
       <c r="I11" s="11"/>
       <c r="L11" s="27"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="45"/>
+      <c r="C12" s="57"/>
       <c r="D12" s="34" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="37">
         <v>0.36</v>
       </c>
-      <c r="F12" s="45"/>
+      <c r="F12" s="57"/>
       <c r="G12" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="54"/>
+      <c r="H12" s="62"/>
       <c r="I12" s="11"/>
       <c r="L12" s="27"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="25" t="s">
         <v>44</v>
       </c>
@@ -1489,12 +1489,12 @@
       <c r="G13" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="54"/>
+      <c r="H13" s="62"/>
       <c r="I13" s="11"/>
       <c r="L13" s="27"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="25" t="s">
         <v>44</v>
       </c>
@@ -1513,16 +1513,16 @@
       <c r="G14" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="54"/>
+      <c r="H14" s="62"/>
       <c r="I14" s="11"/>
       <c r="L14" s="27"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="43" t="s">
+      <c r="A15" s="59"/>
+      <c r="B15" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="55" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="30" t="s">
@@ -1531,38 +1531,38 @@
       <c r="E15" s="42">
         <v>0.52</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="55">
         <v>1</v>
       </c>
-      <c r="G15" s="50" t="s">
+      <c r="G15" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="54"/>
+      <c r="H15" s="62"/>
       <c r="I15" s="11"/>
       <c r="L15" s="27"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
+      <c r="A16" s="59"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
       <c r="D16" s="34" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="37">
         <v>0.12</v>
       </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="54"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="62"/>
       <c r="I16" s="11"/>
       <c r="L16" s="27"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="43" t="s">
+      <c r="A17" s="59"/>
+      <c r="B17" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="55" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="34" t="s">
@@ -1571,55 +1571,55 @@
       <c r="E17" s="36">
         <v>2.14</v>
       </c>
-      <c r="F17" s="43" t="s">
+      <c r="F17" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="50" t="s">
+      <c r="G17" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="54"/>
+      <c r="H17" s="62"/>
       <c r="I17" s="11"/>
       <c r="L17" s="27"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
+      <c r="A18" s="59"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
       <c r="D18" s="34" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="36">
         <v>1.17</v>
       </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="54"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="62"/>
       <c r="I18" s="11" t="s">
         <v>41</v>
       </c>
       <c r="L18" s="27"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
       <c r="D19" s="31" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="36">
         <v>1.99</v>
       </c>
-      <c r="F19" s="45"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="55"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="63"/>
       <c r="I19" s="11"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="59"/>
       <c r="B20" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="55" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="31" t="s">
@@ -1628,7 +1628,7 @@
       <c r="E20" s="35">
         <v>0.34</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="55">
         <v>1</v>
       </c>
       <c r="G20" s="41" t="s">
@@ -1640,18 +1640,18 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="59"/>
       <c r="B21" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="44"/>
+      <c r="C21" s="56"/>
       <c r="D21" s="31" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="36">
         <v>0.05</v>
       </c>
-      <c r="F21" s="44"/>
+      <c r="F21" s="56"/>
       <c r="G21" s="41" t="s">
         <v>50</v>
       </c>
@@ -1661,18 +1661,18 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="45"/>
+      <c r="C22" s="57"/>
       <c r="D22" s="34" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="37">
         <v>0.04</v>
       </c>
-      <c r="F22" s="45"/>
+      <c r="F22" s="57"/>
       <c r="G22" s="41" t="s">
         <v>52</v>
       </c>
@@ -1682,24 +1682,24 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="64"/>
+      <c r="A23" s="69"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="71"/>
     </row>
     <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="55" t="s">
         <v>56</v>
       </c>
       <c r="D24" s="31" t="s">
@@ -1708,7 +1708,7 @@
       <c r="E24" s="3">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="55">
         <v>1</v>
       </c>
       <c r="G24" s="41" t="s">
@@ -1718,16 +1718,16 @@
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
       <c r="D25" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="8">
         <v>15.1</v>
       </c>
-      <c r="F25" s="44"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="41" t="s">
         <v>59</v>
       </c>
@@ -1735,16 +1735,16 @@
       <c r="I25" s="11"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
       <c r="D26" s="29" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="24">
         <v>9.1999999999999993</v>
       </c>
-      <c r="F26" s="45"/>
+      <c r="F26" s="57"/>
       <c r="G26" s="41" t="s">
         <v>58</v>
       </c>
@@ -1753,24 +1753,24 @@
       <c r="J26" s="14"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="62"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="64"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="71"/>
     </row>
     <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="65" t="s">
+      <c r="B28" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="58" t="s">
         <v>61</v>
       </c>
       <c r="D28" s="29" t="s">
@@ -1789,18 +1789,18 @@
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="47"/>
+      <c r="C29" s="59"/>
       <c r="D29" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E29" s="8">
         <v>0.77</v>
       </c>
-      <c r="F29" s="80"/>
+      <c r="F29" s="84"/>
       <c r="G29" s="30" t="s">
         <v>74</v>
       </c>
@@ -1810,322 +1810,322 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="79" t="s">
+      <c r="A30" s="59"/>
+      <c r="B30" s="49" t="s">
         <v>62</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="87" t="s">
+      <c r="D30" s="54" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F30" s="73">
+      <c r="F30" s="46">
         <v>1</v>
       </c>
-      <c r="G30" s="76"/>
-      <c r="H30" s="74"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="47"/>
       <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
-      <c r="B31" s="79" t="s">
+      <c r="A31" s="59"/>
+      <c r="B31" s="49" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="87" t="s">
+      <c r="D31" s="54" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="73">
+      <c r="F31" s="46">
         <v>1</v>
       </c>
-      <c r="G31" s="76"/>
-      <c r="H31" s="74"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="47"/>
       <c r="I31" s="11"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
-      <c r="B32" s="79" t="s">
+      <c r="A32" s="59"/>
+      <c r="B32" s="49" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="87" t="s">
+      <c r="D32" s="54" t="s">
         <v>44</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="73">
+      <c r="F32" s="46">
         <v>1</v>
       </c>
-      <c r="G32" s="76"/>
-      <c r="H32" s="74"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="47"/>
       <c r="I32" s="11"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
-      <c r="B33" s="79" t="s">
+      <c r="A33" s="59"/>
+      <c r="B33" s="49" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="87" t="s">
+      <c r="D33" s="54" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F33" s="73">
+      <c r="F33" s="46">
         <v>2</v>
       </c>
       <c r="G33" s="5"/>
-      <c r="H33" s="74"/>
+      <c r="H33" s="47"/>
       <c r="I33" s="11"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
-      <c r="B34" s="77" t="s">
+      <c r="A34" s="59"/>
+      <c r="B34" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="43" t="s">
+      <c r="C34" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="81" t="s">
+      <c r="D34" s="50" t="s">
         <v>76</v>
       </c>
       <c r="E34" s="8">
         <v>6.99</v>
       </c>
-      <c r="F34" s="49">
+      <c r="F34" s="87">
         <v>1</v>
       </c>
-      <c r="G34" s="50" t="s">
+      <c r="G34" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="H34" s="86"/>
+      <c r="H34" s="53"/>
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
-      <c r="B35" s="78"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="82" t="s">
+      <c r="A35" s="60"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="51" t="s">
         <v>77</v>
       </c>
       <c r="E35" s="24">
         <v>6.49</v>
       </c>
-      <c r="F35" s="78"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="66"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="44"/>
       <c r="I35" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="71"/>
-      <c r="B36" s="75"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="67"/>
-      <c r="I36" s="85"/>
+      <c r="A36" s="79"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="81"/>
+      <c r="G36" s="81"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="82"/>
     </row>
     <row r="37" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="72" t="s">
+      <c r="A37" s="66" t="s">
         <v>11</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="73" t="s">
+      <c r="C37" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="73"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73">
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46">
         <v>1</v>
       </c>
-      <c r="G37" s="73"/>
-      <c r="H37" s="73"/>
-      <c r="I37" s="73"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="69"/>
+      <c r="A38" s="67"/>
       <c r="B38" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="68" t="s">
+      <c r="C38" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="73">
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46">
         <v>1</v>
       </c>
-      <c r="G38" s="73"/>
-      <c r="H38" s="73"/>
-      <c r="I38" s="73"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="69"/>
+      <c r="A39" s="67"/>
       <c r="B39" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="68" t="s">
+      <c r="C39" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73">
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46">
         <v>3</v>
       </c>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
-      <c r="I39" s="73"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="69"/>
+      <c r="A40" s="67"/>
       <c r="B40" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="68" t="s">
+      <c r="C40" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="73"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73">
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46">
         <v>1</v>
       </c>
-      <c r="G40" s="73"/>
-      <c r="H40" s="73"/>
-      <c r="I40" s="73"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="69"/>
+      <c r="A41" s="67"/>
       <c r="B41" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="68" t="s">
+      <c r="C41" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="73"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="73">
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46">
         <v>3</v>
       </c>
-      <c r="G41" s="73"/>
-      <c r="H41" s="73"/>
-      <c r="I41" s="73"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="69"/>
+      <c r="A42" s="67"/>
       <c r="B42" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="68" t="s">
+      <c r="C42" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
-      <c r="F42" s="73">
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46">
         <v>1</v>
       </c>
-      <c r="G42" s="73"/>
-      <c r="H42" s="73"/>
-      <c r="I42" s="73"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="69"/>
+      <c r="A43" s="67"/>
       <c r="B43" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="68" t="s">
+      <c r="C43" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="D43" s="73"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="73">
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46">
         <v>3</v>
       </c>
-      <c r="G43" s="73"/>
-      <c r="H43" s="73"/>
-      <c r="I43" s="73"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="69"/>
+      <c r="A44" s="67"/>
       <c r="B44" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="68" t="s">
+      <c r="C44" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="73">
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46">
         <v>1</v>
       </c>
-      <c r="G44" s="73"/>
-      <c r="H44" s="73"/>
-      <c r="I44" s="73"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="69"/>
+      <c r="A45" s="67"/>
       <c r="B45" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="73">
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46">
         <v>1</v>
       </c>
-      <c r="G45" s="73"/>
-      <c r="H45" s="73"/>
-      <c r="I45" s="73"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="70"/>
+      <c r="A46" s="68"/>
       <c r="B46" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="84" t="s">
+      <c r="C46" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73">
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46">
         <v>1</v>
       </c>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
-      <c r="I46" s="73"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="59"/>
-      <c r="B47" s="60"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="60"/>
-      <c r="I47" s="61"/>
+      <c r="A47" s="76"/>
+      <c r="B47" s="77"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="77"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="77"/>
+      <c r="G47" s="77"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="78"/>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G49" s="33"/>
@@ -2220,8 +2220,10 @@
     <hyperlink ref="G29" r:id="rId37" location="productTechData" xr:uid="{773012C2-973B-43DA-B249-81B7484AA262}"/>
     <hyperlink ref="D34" r:id="rId38" xr:uid="{0DB9BBA3-F2BB-44FE-9D2E-1B319256541B}"/>
     <hyperlink ref="G34" r:id="rId39" xr:uid="{5EFA44F6-4A74-4794-8292-09F8A5D236DB}"/>
+    <hyperlink ref="D7" r:id="rId40" xr:uid="{06564ADF-1A68-4E0B-9289-7E9F642C7421}"/>
+    <hyperlink ref="D9" r:id="rId41" xr:uid="{387E5E29-5F34-4955-8E54-5D0A758BE9C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
designed the schematic for the powerunit and adjusted the component list
</commit_message>
<xml_diff>
--- a/Clock2_0-Comp_List.xlsx
+++ b/Clock2_0-Comp_List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oliwi\Desktop\Project_Ontwerpen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliwier\Desktop\Project_Ontwerpen_1stejaar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C75219A-DBDE-44B0-816C-2559B04EA9CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00F33B2-64C0-4987-AB2B-724BD8955DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
   <si>
     <t>Categorie:</t>
   </si>
@@ -328,6 +328,18 @@
   </si>
   <si>
     <t>C5</t>
+  </si>
+  <si>
+    <t>EXTRA</t>
+  </si>
+  <si>
+    <t>5v,3a capable USB pd unit</t>
+  </si>
+  <si>
+    <t>videolink</t>
+  </si>
+  <si>
+    <t>schroefconnector</t>
   </si>
 </sst>
 </file>
@@ -592,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -638,7 +650,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -653,9 +664,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -672,9 +680,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -729,66 +734,99 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -801,41 +839,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,9 +932,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -963,7 +972,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1069,7 +1078,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1211,7 +1220,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1219,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:L52"/>
+  <dimension ref="A2:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,370 +1277,370 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="21">
         <v>15.99</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="68">
         <v>1</v>
       </c>
-      <c r="G3" s="64" t="s">
+      <c r="G3" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="73"/>
-      <c r="I3" s="61"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="73"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="31" t="s">
+      <c r="A4" s="62"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="26">
         <v>11.99</v>
       </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="62"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="74"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="29" t="s">
+      <c r="A5" s="62"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="27" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="8">
         <v>12.4</v>
       </c>
-      <c r="F5" s="57"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="63"/>
-      <c r="L5" s="27"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="75"/>
+      <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
-      <c r="B6" s="40" t="s">
+      <c r="A6" s="62"/>
+      <c r="B6" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="36">
         <v>1.19</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="37">
         <v>1</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="61"/>
+      <c r="H6" s="73"/>
       <c r="I6" s="6"/>
-      <c r="L6" s="27"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
-      <c r="B7" s="55" t="s">
+      <c r="A7" s="62"/>
+      <c r="B7" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="32">
         <v>0.09</v>
       </c>
-      <c r="F7" s="55">
+      <c r="F7" s="68">
         <v>1</v>
       </c>
-      <c r="G7" s="64" t="s">
+      <c r="G7" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="62"/>
+      <c r="H7" s="74"/>
       <c r="I7" s="11"/>
-      <c r="L7" s="27"/>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="31" t="s">
+      <c r="A8" s="62"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="33">
         <v>0.25</v>
       </c>
-      <c r="F8" s="56"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="62"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="74"/>
       <c r="I8" s="11"/>
-      <c r="L8" s="27"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="31" t="s">
+      <c r="A9" s="62"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="34">
         <v>0.05</v>
       </c>
-      <c r="F9" s="57"/>
-      <c r="G9" s="30" t="s">
+      <c r="F9" s="69"/>
+      <c r="G9" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="62"/>
+      <c r="H9" s="74"/>
       <c r="I9" s="11"/>
-      <c r="L9" s="27"/>
+      <c r="L9" s="25"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="62"/>
+      <c r="B10" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="33">
         <v>0.59</v>
       </c>
-      <c r="F10" s="55">
+      <c r="F10" s="68">
         <v>1</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="62"/>
+      <c r="H10" s="74"/>
       <c r="I10" s="11"/>
-      <c r="L10" s="27"/>
+      <c r="L10" s="25"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="62"/>
+      <c r="B11" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="34" t="s">
+      <c r="C11" s="79"/>
+      <c r="D11" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="33">
         <v>0.27</v>
       </c>
-      <c r="F11" s="56"/>
-      <c r="G11" s="30" t="s">
+      <c r="F11" s="79"/>
+      <c r="G11" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="62"/>
+      <c r="H11" s="74"/>
       <c r="I11" s="11"/>
-      <c r="L11" s="27"/>
+      <c r="L11" s="25"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="23" t="s">
+      <c r="A12" s="62"/>
+      <c r="B12" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="34" t="s">
+      <c r="C12" s="69"/>
+      <c r="D12" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="37">
+      <c r="E12" s="34">
         <v>0.36</v>
       </c>
-      <c r="F12" s="57"/>
-      <c r="G12" s="41" t="s">
+      <c r="F12" s="69"/>
+      <c r="G12" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="62"/>
+      <c r="H12" s="74"/>
       <c r="I12" s="11"/>
-      <c r="L12" s="27"/>
+      <c r="L12" s="25"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="25" t="s">
+      <c r="A13" s="62"/>
+      <c r="B13" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="62"/>
+      <c r="H13" s="74"/>
       <c r="I13" s="11"/>
-      <c r="L13" s="27"/>
+      <c r="L13" s="25"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
-      <c r="B14" s="25" t="s">
+      <c r="A14" s="62"/>
+      <c r="B14" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="62"/>
+      <c r="H14" s="74"/>
       <c r="I14" s="11"/>
-      <c r="L14" s="27"/>
+      <c r="L14" s="25"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="55" t="s">
+      <c r="A15" s="62"/>
+      <c r="B15" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="42">
+      <c r="E15" s="39">
         <v>0.52</v>
       </c>
-      <c r="F15" s="55">
+      <c r="F15" s="68">
         <v>1</v>
       </c>
-      <c r="G15" s="64" t="s">
+      <c r="G15" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="62"/>
+      <c r="H15" s="74"/>
       <c r="I15" s="11"/>
-      <c r="L15" s="27"/>
+      <c r="L15" s="25"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="34" t="s">
+      <c r="A16" s="62"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="37">
+      <c r="E16" s="34">
         <v>0.12</v>
       </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="62"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="74"/>
       <c r="I16" s="11"/>
-      <c r="L16" s="27"/>
+      <c r="L16" s="25"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="55" t="s">
+      <c r="A17" s="62"/>
+      <c r="B17" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E17" s="33">
         <v>2.14</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F17" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="64" t="s">
+      <c r="G17" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="62"/>
+      <c r="H17" s="74"/>
       <c r="I17" s="11"/>
-      <c r="L17" s="27"/>
+      <c r="L17" s="25"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="34" t="s">
+      <c r="A18" s="62"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="33">
         <v>1.17</v>
       </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="62"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="74"/>
       <c r="I18" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="27"/>
+      <c r="L18" s="25"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="31" t="s">
+      <c r="A19" s="62"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="33">
         <v>1.99</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="63"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="75"/>
       <c r="I19" s="11"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
-      <c r="B20" s="20" t="s">
+      <c r="A20" s="62"/>
+      <c r="B20" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="32">
         <v>0.34</v>
       </c>
-      <c r="F20" s="55">
+      <c r="F20" s="68">
         <v>1</v>
       </c>
-      <c r="G20" s="41" t="s">
+      <c r="G20" s="38" t="s">
         <v>46</v>
       </c>
       <c r="H20" s="4"/>
@@ -1640,19 +1649,19 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
-      <c r="B21" s="21" t="s">
+      <c r="A21" s="62"/>
+      <c r="B21" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="56"/>
-      <c r="D21" s="31" t="s">
+      <c r="C21" s="79"/>
+      <c r="D21" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="36">
+      <c r="E21" s="33">
         <v>0.05</v>
       </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="41" t="s">
+      <c r="F21" s="79"/>
+      <c r="G21" s="38" t="s">
         <v>50</v>
       </c>
       <c r="H21" s="9"/>
@@ -1661,19 +1670,19 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="60"/>
-      <c r="B22" s="23" t="s">
+      <c r="A22" s="65"/>
+      <c r="B22" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="57"/>
-      <c r="D22" s="34" t="s">
+      <c r="C22" s="69"/>
+      <c r="D22" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="37">
+      <c r="E22" s="34">
         <v>0.04</v>
       </c>
-      <c r="F22" s="57"/>
-      <c r="G22" s="41" t="s">
+      <c r="F22" s="69"/>
+      <c r="G22" s="38" t="s">
         <v>52</v>
       </c>
       <c r="H22" s="12"/>
@@ -1682,70 +1691,70 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="69"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="71"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="56"/>
     </row>
     <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="29" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="3">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F24" s="55">
+      <c r="F24" s="68">
         <v>1</v>
       </c>
-      <c r="G24" s="41" t="s">
+      <c r="G24" s="38" t="s">
         <v>57</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="31" t="s">
+      <c r="A25" s="62"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="29" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="8">
         <v>15.1</v>
       </c>
-      <c r="F25" s="56"/>
-      <c r="G25" s="41" t="s">
+      <c r="F25" s="79"/>
+      <c r="G25" s="38" t="s">
         <v>59</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="11"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="60"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="29" t="s">
+      <c r="A26" s="65"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="23">
         <v>9.1999999999999993</v>
       </c>
-      <c r="F26" s="57"/>
-      <c r="G26" s="41" t="s">
+      <c r="F26" s="69"/>
+      <c r="G26" s="38" t="s">
         <v>58</v>
       </c>
       <c r="H26" s="10"/>
@@ -1753,402 +1762,541 @@
       <c r="J26" s="14"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="69"/>
-      <c r="B27" s="70"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="71"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="56"/>
     </row>
     <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="27" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="3">
         <v>1.17</v>
       </c>
-      <c r="F28" s="83">
+      <c r="F28" s="63">
         <v>1</v>
       </c>
-      <c r="G28" s="41" t="s">
+      <c r="G28" s="38" t="s">
         <v>73</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="59"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="29" t="s">
+      <c r="C29" s="62"/>
+      <c r="D29" s="27" t="s">
         <v>13</v>
       </c>
       <c r="E29" s="8">
         <v>0.77</v>
       </c>
-      <c r="F29" s="84"/>
-      <c r="G29" s="30" t="s">
+      <c r="F29" s="64"/>
+      <c r="G29" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="H29" s="32"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="59"/>
-      <c r="B30" s="49" t="s">
+      <c r="A30" s="62"/>
+      <c r="B30" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="54" t="s">
+      <c r="D30" s="50" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F30" s="46">
+      <c r="F30" s="43">
         <v>1</v>
       </c>
-      <c r="G30" s="48"/>
-      <c r="H30" s="47"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="44"/>
       <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="59"/>
-      <c r="B31" s="49" t="s">
+      <c r="A31" s="62"/>
+      <c r="B31" s="46" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="54" t="s">
+      <c r="D31" s="50" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="46">
+      <c r="F31" s="43">
         <v>1</v>
       </c>
-      <c r="G31" s="48"/>
-      <c r="H31" s="47"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="44"/>
       <c r="I31" s="11"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
-      <c r="B32" s="49" t="s">
+      <c r="A32" s="62"/>
+      <c r="B32" s="46" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="54" t="s">
+      <c r="D32" s="50" t="s">
         <v>44</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="46">
+      <c r="F32" s="43">
         <v>1</v>
       </c>
-      <c r="G32" s="48"/>
-      <c r="H32" s="47"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="44"/>
       <c r="I32" s="11"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
-      <c r="B33" s="49" t="s">
+      <c r="A33" s="62"/>
+      <c r="B33" s="46" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="54" t="s">
+      <c r="D33" s="50" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F33" s="46">
+      <c r="F33" s="43">
         <v>2</v>
       </c>
       <c r="G33" s="5"/>
-      <c r="H33" s="47"/>
+      <c r="H33" s="44"/>
       <c r="I33" s="11"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
-      <c r="B34" s="85" t="s">
+      <c r="A34" s="62"/>
+      <c r="B34" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="55" t="s">
+      <c r="C34" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="50" t="s">
+      <c r="D34" s="47" t="s">
         <v>76</v>
       </c>
       <c r="E34" s="8">
         <v>6.99</v>
       </c>
-      <c r="F34" s="87">
+      <c r="F34" s="70">
         <v>1</v>
       </c>
-      <c r="G34" s="64" t="s">
+      <c r="G34" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="H34" s="53"/>
+      <c r="H34" s="49"/>
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="60"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="51" t="s">
+      <c r="A35" s="65"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="24">
+      <c r="E35" s="23">
         <v>6.49</v>
       </c>
-      <c r="F35" s="86"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="44"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="41"/>
       <c r="I35" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="79"/>
-      <c r="B36" s="80"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="81"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="82"/>
+      <c r="A36" s="57"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="60"/>
     </row>
     <row r="37" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="76" t="s">
         <v>11</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="46" t="s">
+      <c r="C37" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46">
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43">
         <v>1</v>
       </c>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="67"/>
+      <c r="A38" s="77"/>
       <c r="B38" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="45" t="s">
+      <c r="C38" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46">
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43">
         <v>1</v>
       </c>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="46"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="67"/>
+      <c r="A39" s="77"/>
       <c r="B39" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="45" t="s">
+      <c r="C39" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="46">
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43">
         <v>3</v>
       </c>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="46"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="67"/>
+      <c r="A40" s="77"/>
       <c r="B40" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C40" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46">
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43">
         <v>1</v>
       </c>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="67"/>
+      <c r="A41" s="77"/>
       <c r="B41" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C41" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46">
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43">
         <v>3</v>
       </c>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="46"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="67"/>
+      <c r="A42" s="77"/>
       <c r="B42" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="45" t="s">
+      <c r="C42" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46">
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43">
         <v>1</v>
       </c>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="67"/>
+      <c r="A43" s="77"/>
       <c r="B43" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="45" t="s">
+      <c r="C43" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D43" s="46"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="46">
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43">
         <v>3</v>
       </c>
-      <c r="G43" s="46"/>
-      <c r="H43" s="46"/>
-      <c r="I43" s="46"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="67"/>
+      <c r="A44" s="77"/>
       <c r="B44" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46">
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43">
         <v>1</v>
       </c>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="67"/>
+      <c r="A45" s="77"/>
       <c r="B45" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="45" t="s">
+      <c r="C45" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46">
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43">
         <v>1</v>
       </c>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="68"/>
+      <c r="A46" s="78"/>
       <c r="B46" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="52" t="s">
+      <c r="C46" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46">
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43">
         <v>1</v>
       </c>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="46"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="76"/>
-      <c r="B47" s="77"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="77"/>
-      <c r="G47" s="77"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="78"/>
-    </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G49" s="33"/>
-    </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E51" s="26"/>
-      <c r="G51" s="26"/>
-    </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F52" s="19"/>
+      <c r="A47" s="51"/>
+      <c r="B47" s="52"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
+      <c r="F47" s="52"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="52"/>
+      <c r="I47" s="53"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="86" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="23">
+        <v>13</v>
+      </c>
+      <c r="F48" s="6">
+        <v>1</v>
+      </c>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="77"/>
+      <c r="B49" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="23">
+        <v>0.72</v>
+      </c>
+      <c r="F49" s="11">
+        <v>1</v>
+      </c>
+      <c r="G49" s="9"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="77"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="77"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="84"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="77"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="85"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="77"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="77"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="77"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="77"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="78"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="51"/>
+      <c r="B58" s="52"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52"/>
+      <c r="F58" s="52"/>
+      <c r="G58" s="52"/>
+      <c r="H58" s="52"/>
+      <c r="I58" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="A47:I47"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
+  <mergeCells count="42">
+    <mergeCell ref="A48:A57"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="A3:A22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="F10:F12"/>
     <mergeCell ref="H6:H19"/>
     <mergeCell ref="I3:I5"/>
     <mergeCell ref="G7:G8"/>
@@ -2165,20 +2313,16 @@
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="F17:F19"/>
     <mergeCell ref="G17:G19"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="A3:A22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="A47:I47"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G25" r:id="rId1" xr:uid="{C7C81231-EAB6-4F9D-8DA9-4F8DFA4702DC}"/>
@@ -2222,8 +2366,10 @@
     <hyperlink ref="G34" r:id="rId39" xr:uid="{5EFA44F6-4A74-4794-8292-09F8A5D236DB}"/>
     <hyperlink ref="D7" r:id="rId40" xr:uid="{06564ADF-1A68-4E0B-9289-7E9F642C7421}"/>
     <hyperlink ref="D9" r:id="rId41" xr:uid="{387E5E29-5F34-4955-8E54-5D0A758BE9C3}"/>
+    <hyperlink ref="D48" r:id="rId42" xr:uid="{C0487377-5A73-48FA-B17E-38A258E1C1F0}"/>
+    <hyperlink ref="D49" r:id="rId43" xr:uid="{39567BF0-2109-4DEF-9D52-F3ACF6DA89D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added all necessary footprints
</commit_message>
<xml_diff>
--- a/Clock2_0-Comp_List.xlsx
+++ b/Clock2_0-Comp_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliwier\Desktop\Project_Ontwerpen_1stejaar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00F33B2-64C0-4987-AB2B-724BD8955DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71158F29-559D-41DB-B71D-2EA3A99EF9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12135" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
   <si>
     <t>Categorie:</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t>schroefconnector</t>
+  </si>
+  <si>
+    <t>farnell</t>
   </si>
 </sst>
 </file>
@@ -397,7 +400,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +422,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBA9D0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,14 +619,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -620,9 +632,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -638,28 +647,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -707,9 +704,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -725,9 +719,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -739,105 +730,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -845,6 +737,160 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,6 +965,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFEBA9D0"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1230,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,1026 +1326,1010 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="16">
         <v>15.99</v>
       </c>
-      <c r="F3" s="68">
+      <c r="F3" s="52">
         <v>1</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="81"/>
-      <c r="I3" s="73"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="58"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="29" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="20">
         <v>11.99</v>
       </c>
-      <c r="F4" s="79"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="74"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="59"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="27" t="s">
+      <c r="A5" s="56"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <v>12.4</v>
       </c>
-      <c r="F5" s="69"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="75"/>
-      <c r="L5" s="25"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="60"/>
+      <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="37" t="s">
+      <c r="A6" s="56"/>
+      <c r="B6" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="30">
         <v>1.19</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="31">
         <v>1</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="73"/>
-      <c r="I6" s="6"/>
-      <c r="L6" s="25"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="5"/>
+      <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
-      <c r="B7" s="68" t="s">
+      <c r="A7" s="56"/>
+      <c r="B7" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="26">
         <v>0.09</v>
       </c>
-      <c r="F7" s="68">
+      <c r="F7" s="52">
         <v>1</v>
       </c>
-      <c r="G7" s="71" t="s">
+      <c r="G7" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="74"/>
-      <c r="I7" s="11"/>
-      <c r="L7" s="25"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="9"/>
+      <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="29" t="s">
+      <c r="C8" s="53"/>
+      <c r="D8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="27">
         <v>0.25</v>
       </c>
-      <c r="F8" s="79"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="11"/>
-      <c r="L8" s="25"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="9"/>
+      <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="29" t="s">
+      <c r="A9" s="56"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="28">
         <v>0.05</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="28" t="s">
+      <c r="F9" s="54"/>
+      <c r="G9" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="74"/>
-      <c r="I9" s="11"/>
-      <c r="L9" s="25"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="9"/>
+      <c r="L9" s="19"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="56"/>
+      <c r="B10" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="27">
         <v>0.59</v>
       </c>
-      <c r="F10" s="68">
+      <c r="F10" s="52">
         <v>1</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="74"/>
-      <c r="I10" s="11"/>
-      <c r="L10" s="25"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="9"/>
+      <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
-      <c r="B11" s="20" t="s">
+      <c r="A11" s="56"/>
+      <c r="B11" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="31" t="s">
+      <c r="C11" s="53"/>
+      <c r="D11" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="27">
         <v>0.27</v>
       </c>
-      <c r="F11" s="79"/>
-      <c r="G11" s="28" t="s">
+      <c r="F11" s="53"/>
+      <c r="G11" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="74"/>
-      <c r="I11" s="11"/>
-      <c r="L11" s="25"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="9"/>
+      <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="56"/>
+      <c r="B12" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="31" t="s">
+      <c r="C12" s="54"/>
+      <c r="D12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="28">
         <v>0.36</v>
       </c>
-      <c r="F12" s="69"/>
-      <c r="G12" s="38" t="s">
+      <c r="F12" s="54"/>
+      <c r="G12" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="74"/>
-      <c r="I12" s="11"/>
-      <c r="L12" s="25"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="9"/>
+      <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
-      <c r="B13" s="24" t="s">
+      <c r="A13" s="56"/>
+      <c r="B13" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="74"/>
-      <c r="I13" s="11"/>
-      <c r="L13" s="25"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="9"/>
+      <c r="L13" s="19"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="56"/>
+      <c r="B14" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="74"/>
-      <c r="I14" s="11"/>
-      <c r="L14" s="25"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="9"/>
+      <c r="L14" s="19"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
-      <c r="B15" s="68" t="s">
+      <c r="A15" s="56"/>
+      <c r="B15" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="39">
+      <c r="E15" s="33">
         <v>0.52</v>
       </c>
-      <c r="F15" s="68">
+      <c r="F15" s="52">
         <v>1</v>
       </c>
-      <c r="G15" s="71" t="s">
+      <c r="G15" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="74"/>
-      <c r="I15" s="11"/>
-      <c r="L15" s="25"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="9"/>
+      <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="31" t="s">
+      <c r="A16" s="56"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="28">
         <v>0.12</v>
       </c>
-      <c r="F16" s="69"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="11"/>
-      <c r="L16" s="25"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="9"/>
+      <c r="L16" s="19"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
-      <c r="B17" s="68" t="s">
+      <c r="A17" s="56"/>
+      <c r="B17" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="27">
         <v>2.14</v>
       </c>
-      <c r="F17" s="68" t="s">
+      <c r="F17" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="71" t="s">
+      <c r="G17" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="74"/>
-      <c r="I17" s="11"/>
-      <c r="L17" s="25"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="9"/>
+      <c r="L17" s="19"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="31" t="s">
+      <c r="C18" s="53"/>
+      <c r="D18" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="27">
         <v>1.17</v>
       </c>
-      <c r="F18" s="79"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="11" t="s">
+      <c r="F18" s="53"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="25"/>
+      <c r="L18" s="19"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="62"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="29" t="s">
+      <c r="A19" s="56"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="27">
         <v>1.99</v>
       </c>
-      <c r="F19" s="69"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="11"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="56"/>
+      <c r="B20" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="68" t="s">
+      <c r="C20" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="26">
         <v>0.34</v>
       </c>
-      <c r="F20" s="68">
+      <c r="F20" s="52">
         <v>1</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G20" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="6" t="s">
+      <c r="H20" s="3"/>
+      <c r="I20" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
-      <c r="B21" s="20" t="s">
+      <c r="A21" s="56"/>
+      <c r="B21" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="29" t="s">
+      <c r="C21" s="53"/>
+      <c r="D21" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="27">
         <v>0.05</v>
       </c>
-      <c r="F21" s="79"/>
-      <c r="G21" s="38" t="s">
+      <c r="F21" s="53"/>
+      <c r="G21" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="11" t="s">
+      <c r="H21" s="7"/>
+      <c r="I21" s="9" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="65"/>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="57"/>
+      <c r="B22" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="31" t="s">
+      <c r="C22" s="54"/>
+      <c r="D22" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="34">
+      <c r="E22" s="28">
         <v>0.04</v>
       </c>
-      <c r="F22" s="69"/>
-      <c r="G22" s="38" t="s">
+      <c r="F22" s="54"/>
+      <c r="G22" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="13" t="s">
+      <c r="H22" s="10"/>
+      <c r="I22" s="11" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="56"/>
+      <c r="A23" s="63"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="65"/>
     </row>
     <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="68" t="s">
+      <c r="C24" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F24" s="68">
+      <c r="F24" s="52">
         <v>1</v>
       </c>
-      <c r="G24" s="38" t="s">
+      <c r="G24" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="6"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="62"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="29" t="s">
+      <c r="C25" s="53"/>
+      <c r="D25" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="6">
         <v>15.1</v>
       </c>
-      <c r="F25" s="79"/>
-      <c r="G25" s="38" t="s">
+      <c r="F25" s="53"/>
+      <c r="G25" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="11"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="65"/>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="27" t="s">
+      <c r="A26" s="57"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="17">
         <v>9.1999999999999993</v>
       </c>
-      <c r="F26" s="69"/>
-      <c r="G26" s="38" t="s">
+      <c r="F26" s="54"/>
+      <c r="G26" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="14"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="12"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="56"/>
+      <c r="A27" s="63"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="65"/>
     </row>
     <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="61" t="s">
+      <c r="C28" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>1.17</v>
       </c>
-      <c r="F28" s="63">
+      <c r="F28" s="74">
         <v>1</v>
       </c>
-      <c r="G28" s="38" t="s">
+      <c r="G28" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="6"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
-      <c r="B29" s="15" t="s">
+      <c r="A29" s="56"/>
+      <c r="B29" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="27" t="s">
+      <c r="C29" s="56"/>
+      <c r="D29" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="6">
         <v>0.77</v>
       </c>
-      <c r="F29" s="64"/>
-      <c r="G29" s="28" t="s">
+      <c r="F29" s="75"/>
+      <c r="G29" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="H29" s="30"/>
-      <c r="I29" s="13" t="s">
+      <c r="H29" s="24"/>
+      <c r="I29" s="11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
-      <c r="B30" s="46" t="s">
+      <c r="A30" s="56"/>
+      <c r="B30" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="50" t="s">
+      <c r="D30" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F30" s="36">
+        <v>1</v>
+      </c>
+      <c r="G30" s="38"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="56"/>
+      <c r="B31" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" s="36">
+        <v>1</v>
+      </c>
+      <c r="G31" s="38"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="56"/>
+      <c r="B32" s="89" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E32" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F30" s="43">
+      <c r="F32" s="36">
         <v>1</v>
       </c>
-      <c r="G30" s="45"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="11"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
-      <c r="B31" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="50" t="s">
+      <c r="G32" s="38"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="56"/>
+      <c r="B33" s="89" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E33" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="43">
+      <c r="F33" s="36">
+        <v>2</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="56"/>
+      <c r="B34" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="6">
+        <v>6.99</v>
+      </c>
+      <c r="F34" s="77">
         <v>1</v>
       </c>
-      <c r="G31" s="45"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="11"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
-      <c r="B32" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="18" t="s">
+      <c r="G34" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" s="41"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="57"/>
+      <c r="B35" s="92"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="17">
+        <v>6.49</v>
+      </c>
+      <c r="F35" s="76"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="70"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="73"/>
+    </row>
+    <row r="37" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="93" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36">
+        <v>1</v>
+      </c>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="47"/>
+      <c r="B38" s="94" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36">
+        <v>1</v>
+      </c>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="47"/>
+      <c r="B39" s="94" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36">
+        <v>3</v>
+      </c>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="47"/>
+      <c r="B40" s="94" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36">
+        <v>1</v>
+      </c>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="47"/>
+      <c r="B41" s="94" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36">
+        <v>3</v>
+      </c>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="36"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="47"/>
+      <c r="B42" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36">
+        <v>1</v>
+      </c>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="47"/>
+      <c r="B43" s="94" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36">
+        <v>3</v>
+      </c>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="47"/>
+      <c r="B44" s="94" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36">
+        <v>1</v>
+      </c>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="47"/>
+      <c r="B45" s="94" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36">
+        <v>1</v>
+      </c>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="48"/>
+      <c r="B46" s="95" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36">
+        <v>1</v>
+      </c>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="36"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="49"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="51"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="96" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="17">
+        <v>13</v>
+      </c>
+      <c r="F48" s="5">
+        <v>1</v>
+      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="47"/>
+      <c r="B49" s="85" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F32" s="43">
+      <c r="D49" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="17">
+        <v>0.72</v>
+      </c>
+      <c r="F49" s="9">
         <v>1</v>
       </c>
-      <c r="G32" s="45"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="11"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
-      <c r="B33" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F33" s="43">
-        <v>2</v>
-      </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="11"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="62"/>
-      <c r="B34" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="E34" s="8">
-        <v>6.99</v>
-      </c>
-      <c r="F34" s="70">
-        <v>1</v>
-      </c>
-      <c r="G34" s="71" t="s">
-        <v>80</v>
-      </c>
-      <c r="H34" s="49"/>
-      <c r="I34" s="6"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="65"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="23">
-        <v>6.49</v>
-      </c>
-      <c r="F35" s="67"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="57"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="60"/>
-    </row>
-    <row r="37" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="76" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43">
-        <v>1</v>
-      </c>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="77"/>
-      <c r="B38" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43">
-        <v>1</v>
-      </c>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="77"/>
-      <c r="B39" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43">
-        <v>3</v>
-      </c>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="77"/>
-      <c r="B40" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43">
-        <v>1</v>
-      </c>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="77"/>
-      <c r="B41" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43">
-        <v>3</v>
-      </c>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="77"/>
-      <c r="B42" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43">
-        <v>1</v>
-      </c>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="77"/>
-      <c r="B43" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43">
-        <v>3</v>
-      </c>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="77"/>
-      <c r="B44" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43">
-        <v>1</v>
-      </c>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="77"/>
-      <c r="B45" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43">
-        <v>1</v>
-      </c>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="78"/>
-      <c r="B46" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43">
-        <v>1</v>
-      </c>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="51"/>
-      <c r="B47" s="52"/>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="52"/>
-      <c r="F47" s="52"/>
-      <c r="G47" s="52"/>
-      <c r="H47" s="52"/>
-      <c r="I47" s="53"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="76" t="s">
-        <v>101</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="D48" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="E48" s="23">
-        <v>13</v>
-      </c>
-      <c r="F48" s="6">
-        <v>1</v>
-      </c>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="77"/>
-      <c r="B49" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="23">
-        <v>0.72</v>
-      </c>
-      <c r="F49" s="11">
-        <v>1</v>
-      </c>
-      <c r="G49" s="9"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="77"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="77"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="84"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="77"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="85"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="77"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="77"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="77"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
+      <c r="A55" s="47"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="77"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
+      <c r="A56" s="47"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="78"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
+      <c r="A57" s="48"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="51"/>
-      <c r="B58" s="52"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="52"/>
-      <c r="E58" s="52"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="52"/>
-      <c r="H58" s="52"/>
-      <c r="I58" s="53"/>
+      <c r="A58" s="49"/>
+      <c r="B58" s="50"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="50"/>
+      <c r="I58" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A48:A57"/>
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="A3:A22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="F10:F12"/>
     <mergeCell ref="H6:H19"/>
     <mergeCell ref="I3:I5"/>
     <mergeCell ref="G7:G8"/>
@@ -2313,6 +2346,22 @@
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="F17:F19"/>
     <mergeCell ref="G17:G19"/>
+    <mergeCell ref="A3:A22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="A48:A57"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="F24:F26"/>
     <mergeCell ref="A47:I47"/>
     <mergeCell ref="A27:I27"/>
     <mergeCell ref="A36:I36"/>
@@ -2368,8 +2417,10 @@
     <hyperlink ref="D9" r:id="rId41" xr:uid="{387E5E29-5F34-4955-8E54-5D0A758BE9C3}"/>
     <hyperlink ref="D48" r:id="rId42" xr:uid="{C0487377-5A73-48FA-B17E-38A258E1C1F0}"/>
     <hyperlink ref="D49" r:id="rId43" xr:uid="{39567BF0-2109-4DEF-9D52-F3ACF6DA89D4}"/>
+    <hyperlink ref="D30" r:id="rId44" xr:uid="{E9221F16-154C-40F9-B709-AB5887C413D1}"/>
+    <hyperlink ref="D31" r:id="rId45" xr:uid="{1C5E53F9-460B-45E4-B1A3-C60E9A23F5F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId44"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>